<commit_message>
Correct error in Diagnostic excel file
</commit_message>
<xml_diff>
--- a/(3) Diagnostic of Transformed Data.xlsx
+++ b/(3) Diagnostic of Transformed Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackh\OneDrive\Documents\GitHub\Project-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackh\OneDrive\Documents\GitHub\Project-1\Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{435AA443-B1CF-4239-BA51-27374566EC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF5CA7F-5CF2-4FF5-9303-9932D60632FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{570A10A8-9F99-47ED-B2D6-B6BFA2AA47D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{570A10A8-9F99-47ED-B2D6-B6BFA2AA47D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +569,7 @@
         <v>0.254</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +581,7 @@
         <v>-2.35E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>